<commit_message>
NBN FTTP tab working
</commit_message>
<xml_diff>
--- a/Datatypes.xlsx
+++ b/Datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27390" windowHeight="17580"/>
+    <workbookView windowWidth="15525" windowHeight="17580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
   <si>
     <t>data types</t>
   </si>
@@ -62,6 +62,15 @@
     <t>button</t>
   </si>
   <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>subCategories</t>
+  </si>
+  <si>
     <t>info</t>
   </si>
   <si>
@@ -90,6 +99,12 @@
   </si>
   <si>
     <t>radio-conditional</t>
+  </si>
+  <si>
+    <t>tabs</t>
+  </si>
+  <si>
+    <t>btn-selection</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1267,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="E8:N19"/>
+  <dimension ref="E8:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1263,6 +1278,7 @@
     <col min="5" max="5" width="21.8571428571429" customWidth="1"/>
     <col min="6" max="13" width="10.7142857142857" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.14285714285714" style="1"/>
+    <col min="16" max="16" width="14.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="8" spans="5:5">
@@ -1270,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="5:14">
+    <row r="11" spans="5:17">
       <c r="E11" t="s">
         <v>1</v>
       </c>
@@ -1300,159 +1316,189 @@
       </c>
       <c r="N11" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="O11" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="5:11">
       <c r="E12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="5:11">
       <c r="E13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="5:11">
       <c r="E14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="5:14">
       <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="5:11">
       <c r="E16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>15</v>
+      </c>
       <c r="H16" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="5:13">
       <c r="E17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>15</v>
+      </c>
       <c r="H17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="5:11">
       <c r="E18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="5:13">
       <c r="E19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="5:16">
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" t="s">
+        <v>15</v>
+      </c>
+      <c r="P20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="5:17">
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21"/>
+      <c r="Q21" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>